<commit_message>
✨ feat: Desafio Web Scraping, Tratamentos, Análises; Web Scraping finalizado; Tratamento finalizado; Análise em andamento
</commit_message>
<xml_diff>
--- a/2025-1S-1CD/Sprint2/web_scraping/updated_scraping_propeties/casinhas.xlsx
+++ b/2025-1S-1CD/Sprint2/web_scraping/updated_scraping_propeties/casinhas.xlsx
@@ -473,8 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lote/Terreno para comprar em
-Industrial, Alumínio</t>
+          <t>Rodovia Raposo Tavares</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -512,8 +511,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque Residencial Cidade Universitária, Ribeirão Preto</t>
+          <t>Rua Hermenegildo D'Andréa</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -554,8 +552,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Loteamento Villa Branca, Jacareí</t>
+          <t>Avenida das Letras</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -596,8 +593,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Vila Camilópolis, Santo André</t>
+          <t>Rua Clara</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -638,8 +634,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Casa de condomínio para comprar em
-Balneário Praia do Pernambuco, Guarujá</t>
+          <t>Avenida Moysés Sayão</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -680,8 +675,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Parque dos Lagos, Ribeirão Preto</t>
+          <t>Alameda Francisco Cristófani</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -720,12 +714,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Casa para comprar em
-Jardim Campos Verdes, Londrina</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t>R$ 455.000</t>
@@ -764,8 +753,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Tibiriçá, Santo André</t>
+          <t>Rua Adelmar Tavares</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -806,8 +794,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Parque Jaçatuba, Santo André</t>
+          <t>Rua Icó</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -848,8 +835,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Rio Pequeno, São Paulo</t>
+          <t>Travessa Herval D'Oeste</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -890,8 +876,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Conceição, Osasco</t>
+          <t>Rua Pernambucana</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -932,8 +917,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Industrial, Anápolis</t>
+          <t>Rua Ferroviária Bráulio dos Reis</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -974,8 +958,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Jardim Parque Jupiá, Piracicaba</t>
+          <t>Rua Adolfo Rodrigues</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1016,8 +999,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Casa de condomínio para comprar em
-Piracangaguá II, Taubaté</t>
+          <t>Avenida Virgilio Cardoso Pinna</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1058,8 +1040,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Utinga, Santo André</t>
+          <t>Rua Ancara</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1100,8 +1081,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Paraíso, Santo André</t>
+          <t>Rua Gamboa</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1142,8 +1122,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Fazenda/Sítio/Chácara para comprar em
-Chácaras Fernão Dias, Atibaia</t>
+          <t>Rua dos Cravos</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1181,8 +1160,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Utinga, Santo André</t>
+          <t>Rua Oslo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1223,8 +1201,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Cecília Maria, Santo André</t>
+          <t>Rua Anhanga</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1265,8 +1242,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Centro, Jacareí</t>
+          <t>Rua Vicentina</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1307,8 +1283,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Sumaré, São Paulo</t>
+          <t>Rua Bernardo da Veiga</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1349,8 +1324,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Firmiano Pinto, São Paulo</t>
+          <t>Avenida Doutor Ricardo Jafet</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1388,12 +1362,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Casa para comprar em
-Conjunto Habitacional Jardim das Palmeiras, Ribeirão Preto</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
           <t>R$ 290.000</t>
@@ -1431,8 +1400,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Vila Lutécia, Santo André</t>
+          <t>Rua Júlio Verne</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1473,8 +1441,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Vila Rica, Santo André</t>
+          <t>Rua Vasco Fernandes Coutinho</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1515,8 +1482,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Vila Pires, Santo André</t>
+          <t>Rua Coroados</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1557,8 +1523,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Leonor, São Paulo</t>
+          <t>Rua José Yazigi</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1599,8 +1564,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Antonieta, São Paulo</t>
+          <t>Rua Refinaria Mataripe</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1641,8 +1605,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Vila Guarani, Santo André</t>
+          <t>Rua Odete</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1681,12 +1644,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Fazenda Rio Preto, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
           <t>R$ 134.400</t>
@@ -1722,8 +1680,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Brooklin Paulista, São Paulo</t>
+          <t>Avenida Nova Independência</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1764,8 +1721,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Raposo Tavares, São Paulo</t>
+          <t>Rua Bartolomeu Caporali</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1806,8 +1762,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Silveira, Santo André</t>
+          <t>Avenida Dom Pedro I</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1848,8 +1803,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Prédio/Edificio inteiro para comprar em
-Vila Guarani, Santo André</t>
+          <t>Avenida Valentim Magalhães</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1889,8 +1843,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Setor Lago dos Buritis, Anápolis</t>
+          <t>Rua das Garças</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1931,8 +1884,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque Oratório, Santo André</t>
+          <t>Avenida Araucária</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1973,8 +1925,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila América, Santo André</t>
+          <t>Rua Nilo Peçanha</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2015,8 +1966,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Botânico, Uberlândia</t>
+          <t>Avenida Vereador Carlito Cordeiro</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2057,8 +2007,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Bosque dos Eucaliptos, São José dos Campos</t>
+          <t>Rua Itanhomi</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2097,12 +2046,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Parque das Flores I, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
           <t>R$ 512.420</t>
@@ -2138,8 +2082,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque Marajoara, Santo André</t>
+          <t>Rua Rogério Giorgi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2180,8 +2123,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Chácara Esperia, Piracicaba</t>
+          <t>Rua Rio Grande do Sul</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2222,8 +2164,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Sumaré, São Paulo</t>
+          <t>Rua Bernardo da Veiga</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2264,8 +2205,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Jardim Tupanci, Barueri</t>
+          <t>Rua Werner Goldberg</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2306,8 +2246,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Pires, Santo André</t>
+          <t>Rua Clélia</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2348,8 +2287,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Casa de condomínio para comprar em
-Jardim Celeste, São Paulo</t>
+          <t>Rua Sebastião Annunciatto</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2389,8 +2327,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Graciosa, São Paulo</t>
+          <t>Avenida Professor Luiz Ignácio Anhaia Mello</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2431,8 +2368,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-São João Batista, São João Batista</t>
+          <t>Estrada Geral Vargem Pequena</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2470,12 +2406,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Casa de condomínio para comprar em
-Piracangaguá, Taubaté</t>
-        </is>
-      </c>
+      <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
           <t>R$ 1.250.000</t>
@@ -2514,8 +2445,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Prédio/Edificio inteiro para comprar em
-Casa Branca, Santo André</t>
+          <t>Avenida Firestone</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2555,8 +2485,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Vila Pires, Santo André</t>
+          <t>Rua Caquito</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2597,8 +2526,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Pinheiros, São Paulo</t>
+          <t>Rua Doutor Virgílio de Carvalho Pinto</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2639,8 +2567,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Prudente, São Paulo</t>
+          <t>Rua Cavour</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2679,12 +2606,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Apartamento para comprar em
-Recreio Anhangüera, Ribeirão Preto</t>
-        </is>
-      </c>
+      <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
           <t>R$ 165.000</t>
@@ -2723,8 +2645,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Parque Oratório, Santo André</t>
+          <t>Rua Tangânica</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2763,12 +2684,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Casa de condomínio para comprar em
-Vila Formosa, São Paulo</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
           <t>R$ 508.000</t>
@@ -2805,12 +2721,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Jardim Arroyo, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
           <t>R$ 180.000</t>
@@ -2846,8 +2757,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Bosque dos Eucaliptos, São José dos Campos</t>
+          <t>Rua Ministro José Geraldo Rodrigues Alkmin</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2888,8 +2798,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Vila Assunção, Santo André</t>
+          <t>Travessa Apeninos</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2930,8 +2839,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Casa de condomínio para comprar em
-Vila Antonieta, São Paulo</t>
+          <t>Rua Refinaria Mataripe</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2972,8 +2880,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Jardim Santo André, São Paulo</t>
+          <t>Rua São João</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -3014,8 +2921,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Carijós, Indaial</t>
+          <t>Rua 30 de Outubro</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -3056,8 +2962,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Prudente, São Paulo</t>
+          <t>Rua Ibitirama</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3098,8 +3003,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Parque das Nações, Santo André</t>
+          <t>Rua Coréia</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3140,8 +3044,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Condomínio Maracanã, Santo André</t>
+          <t>Rua Alberto de Oliveira</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3182,8 +3085,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Ana Maria, Santo André</t>
+          <t>Rua Raul Pompéia</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3222,12 +3124,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Residencial Gaivota II, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
           <t>R$ 585.000</t>
@@ -3263,8 +3160,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Vila Gomes, São Paulo</t>
+          <t>Rua Adriano Theodósio Serra</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3305,8 +3201,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Humaitá, Santo André</t>
+          <t>Rua Conde Juliano</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3347,8 +3242,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Nova Petrópolis, São Bernardo do Campo</t>
+          <t>Alameda Princeza Januária</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3389,8 +3283,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Sanches, São José dos Campos</t>
+          <t>Rua Abolição</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3431,8 +3324,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Edi, São Paulo</t>
+          <t>Rua Domingos Garcia Velho</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3473,8 +3365,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque João Ramalho, Santo André</t>
+          <t>Rua Piracanjuba</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3515,8 +3406,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Lote/Terreno para comprar em
-Vila Germer, Timbó</t>
+          <t>Rua Quintino Bocaiúva</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3552,12 +3442,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Fazenda Rio Preto, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A76" t="inlineStr"/>
       <c r="B76" t="inlineStr">
         <is>
           <t>R$ 110.000</t>
@@ -3593,8 +3478,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque Marajoara, Santo André</t>
+          <t>Rua Daniel Berg</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3635,8 +3519,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Fazenda/Sítio/Chácara para comprar em
-Distrito Industrial, Araxá</t>
+          <t>Rodovia BR-262</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3674,8 +3557,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Jardim Caiapiá, Cotia</t>
+          <t>Estrada Manoel Lages do Chao</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3716,8 +3598,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila América, Santo André</t>
+          <t>Rua Onze de Agosto</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3758,8 +3639,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Homero Thon, Santo André</t>
+          <t>Rua Campo Grande</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3800,8 +3680,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Lote/Terreno para comprar em
-Arapongas, Indaial</t>
+          <t>Rua Augusto Maass</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3837,12 +3716,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Fazenda Rio Preto, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr">
         <is>
           <t>R$ 110.000</t>
@@ -3876,12 +3750,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Apartamento para comprar em
-Vila Galvão, Guarulhos</t>
-        </is>
-      </c>
+      <c r="A84" t="inlineStr"/>
       <c r="B84" t="inlineStr">
         <is>
           <t>R$ 296.000</t>
@@ -3920,8 +3789,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Lote/Terreno para comprar em
-Jardim Concórdia, Toledo</t>
+          <t>Rua Leopoldo Schmidt</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3957,12 +3825,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Apartamento para comprar em
-Centro, Timbó</t>
-        </is>
-      </c>
+      <c r="A86" t="inlineStr"/>
       <c r="B86" t="inlineStr">
         <is>
           <t>R$ 549.900</t>
@@ -4000,8 +3863,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Leonor, São Paulo</t>
+          <t>Rua Jandiro Joaquim Pereira</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4042,8 +3904,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Paulista, Campo Grande</t>
+          <t>Rua João Maluf</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -4083,8 +3944,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Scarpelli, Santo André</t>
+          <t>Travessa João Mendes</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -4125,8 +3985,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Manoel Penna, Ribeirão Preto</t>
+          <t>Rua Alfredo Faria de Souza</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -4167,8 +4026,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Jardim Brasil (Zona Norte), São Paulo</t>
+          <t>Avenida Mendes da Rocha</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -4207,12 +4065,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Lote/Terreno para comprar em
-Residencial Maria Clara, São José do Rio Preto</t>
-        </is>
-      </c>
+      <c r="A92" t="inlineStr"/>
       <c r="B92" t="inlineStr">
         <is>
           <t>R$ 93.000</t>
@@ -4246,12 +4099,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Casa para comprar em
-Jardim Jandira, Bauru</t>
-        </is>
-      </c>
+      <c r="A93" t="inlineStr"/>
       <c r="B93" t="inlineStr">
         <is>
           <t>R$ 380.000</t>
@@ -4290,8 +4138,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Lote/Terreno para comprar em
-Vila Germer, Timbó</t>
+          <t>Rua Quintino Bocaiúva</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -4329,8 +4176,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Casa de condomínio para comprar em
-Vila Matilde, São Paulo</t>
+          <t>Rua Eugênia de Carvalho</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -4371,8 +4217,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Tibiriçá, Santo André</t>
+          <t>Rua Álvaro Lins</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -4413,8 +4258,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Santa Maria, São Paulo</t>
+          <t>Rua Doutor Fleury Silveira</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -4454,8 +4298,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque dos Pirineus, Anápolis</t>
+          <t>Rua PP 8</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -4496,8 +4339,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Parque Gerassi, Santo André</t>
+          <t>Rua Kalil Filho</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -4538,8 +4380,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Residencial Campos do Jordão, Anápolis</t>
+          <t>Rua CJ 04</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -4580,8 +4421,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Vila Andrade, São Paulo</t>
+          <t>Rua José de Oliveira Coelho</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -4622,8 +4462,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Cobertura para comprar em
-Vila Marina, Santo André</t>
+          <t>Rua das Azaléas</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -4664,8 +4503,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Tamboré, Barueri</t>
+          <t>Avenida Aruanã</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -4706,8 +4544,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Paraíso, Santo André</t>
+          <t>Travessa Cantareira</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -4748,8 +4585,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Apartamento para comprar em
-Santa Mônica, Uberlândia</t>
+          <t>Rua Antônio Salviano de Rezende</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -4790,8 +4626,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Casa para comprar em
-Jardim Aricanduva, São Paulo</t>
+          <t>Avenida Francisco José Resende</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">

</xml_diff>